<commit_message>
Addressed code review changes
</commit_message>
<xml_diff>
--- a/test/resources/definitionsFiles/fe-automation-definition-v21_RDM-4648_dynamiclists.xlsx
+++ b/test/resources/definitionsFiles/fe-automation-definition-v21_RDM-4648_dynamiclists.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohammedanaskhatri/project/ccd-case-management-web/test/resources/definitionsFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F969791-62E9-C141-B5DF-219A1F8CB5B7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB48B53-B0AF-894A-A83A-972E14FFA7FD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19220" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19220" firstSheet="8" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3562" uniqueCount="683">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3566" uniqueCount="683">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -5522,8 +5522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:AD106"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView showGridLines="0" topLeftCell="A6" zoomScale="218" zoomScaleNormal="218" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5542,7 +5542,8 @@
     <col min="14" max="14" width="22" style="142" customWidth="1"/>
     <col min="15" max="15" width="42.5" style="22" customWidth="1"/>
     <col min="16" max="16" width="28.33203125" style="22" customWidth="1"/>
-    <col min="17" max="29" width="8.83203125" style="22" customWidth="1"/>
+    <col min="17" max="17" width="26.33203125" style="22" customWidth="1"/>
+    <col min="18" max="29" width="8.83203125" style="22" customWidth="1"/>
     <col min="30" max="257" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -12847,10 +12848,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:K95"/>
+  <dimension ref="A1:K96"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -13286,10 +13287,10 @@
       </c>
       <c r="B19" s="7"/>
       <c r="C19" s="8" t="s">
-        <v>275</v>
+        <v>396</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>276</v>
+        <v>679</v>
       </c>
       <c r="E19" t="s">
         <v>271</v>
@@ -13303,16 +13304,16 @@
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
     </row>
-    <row r="20" spans="1:11" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="10">
         <v>42736</v>
       </c>
-      <c r="B20" s="10"/>
-      <c r="C20" s="57" t="s">
+      <c r="B20" s="7"/>
+      <c r="C20" s="8" t="s">
         <v>275</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E20" t="s">
         <v>271</v>
@@ -13320,17 +13321,22 @@
       <c r="F20" s="8" t="s">
         <v>244</v>
       </c>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
     </row>
     <row r="21" spans="1:11" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="10">
         <v>42736</v>
       </c>
       <c r="B21" s="10"/>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="57" t="s">
         <v>275</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E21" t="s">
         <v>271</v>
@@ -13338,11 +13344,6 @@
       <c r="F21" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="G21" s="42"/>
-      <c r="H21" s="42"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="42"/>
-      <c r="K21" s="42"/>
     </row>
     <row r="22" spans="1:11" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="10">
@@ -13353,7 +13354,7 @@
         <v>275</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>679</v>
+        <v>278</v>
       </c>
       <c r="E22" t="s">
         <v>271</v>
@@ -13375,8 +13376,8 @@
       <c r="C23" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="D23" s="57" t="s">
-        <v>366</v>
+      <c r="D23" s="8" t="s">
+        <v>679</v>
       </c>
       <c r="E23" t="s">
         <v>271</v>
@@ -13384,54 +13385,54 @@
       <c r="F23" s="8" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" s="93" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="110">
-        <v>42736</v>
-      </c>
-      <c r="B24" s="92"/>
-      <c r="C24" s="111" t="s">
+      <c r="G23" s="42"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="42"/>
+      <c r="J23" s="42"/>
+      <c r="K23" s="42"/>
+    </row>
+    <row r="24" spans="1:11" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B24" s="10"/>
+      <c r="C24" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="D24" s="111" t="s">
+      <c r="D24" s="57" t="s">
+        <v>366</v>
+      </c>
+      <c r="E24" t="s">
+        <v>271</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" s="93" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="110">
+        <v>42736</v>
+      </c>
+      <c r="B25" s="92"/>
+      <c r="C25" s="111" t="s">
+        <v>275</v>
+      </c>
+      <c r="D25" s="111" t="s">
         <v>474</v>
       </c>
-      <c r="E24" s="93" t="s">
+      <c r="E25" s="93" t="s">
         <v>271</v>
       </c>
-      <c r="F24" s="111" t="s">
+      <c r="F25" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="G24" s="92"/>
-      <c r="H24" s="92"/>
-      <c r="I24" s="92"/>
-      <c r="J24" s="92"/>
-      <c r="K24" s="92"/>
-    </row>
-    <row r="25" spans="1:11" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B25" s="10"/>
-      <c r="C25" s="86" t="s">
-        <v>285</v>
-      </c>
-      <c r="D25" s="57" t="s">
-        <v>296</v>
-      </c>
-      <c r="E25" t="s">
-        <v>271</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="G25" s="42"/>
-      <c r="H25" s="42"/>
-      <c r="I25" s="42"/>
-      <c r="J25" s="42"/>
-      <c r="K25" s="42"/>
-    </row>
-    <row r="26" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G25" s="92"/>
+      <c r="H25" s="92"/>
+      <c r="I25" s="92"/>
+      <c r="J25" s="92"/>
+      <c r="K25" s="92"/>
+    </row>
+    <row r="26" spans="1:11" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="10">
         <v>42736</v>
       </c>
@@ -13440,7 +13441,7 @@
         <v>285</v>
       </c>
       <c r="D26" s="57" t="s">
-        <v>314</v>
+        <v>296</v>
       </c>
       <c r="E26" t="s">
         <v>271</v>
@@ -13454,7 +13455,7 @@
       <c r="J26" s="42"/>
       <c r="K26" s="42"/>
     </row>
-    <row r="27" spans="1:11" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="10">
         <v>42736</v>
       </c>
@@ -13463,7 +13464,7 @@
         <v>285</v>
       </c>
       <c r="D27" s="57" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E27" t="s">
         <v>271</v>
@@ -13481,12 +13482,12 @@
       <c r="A28" s="10">
         <v>42736</v>
       </c>
-      <c r="B28" s="7"/>
+      <c r="B28" s="10"/>
       <c r="C28" s="86" t="s">
         <v>285</v>
       </c>
       <c r="D28" s="57" t="s">
-        <v>454</v>
+        <v>311</v>
       </c>
       <c r="E28" t="s">
         <v>271</v>
@@ -13508,8 +13509,8 @@
       <c r="C29" s="86" t="s">
         <v>285</v>
       </c>
-      <c r="D29" s="173" t="s">
-        <v>548</v>
+      <c r="D29" s="57" t="s">
+        <v>454</v>
       </c>
       <c r="E29" t="s">
         <v>271</v>
@@ -13523,51 +13524,51 @@
       <c r="J29" s="42"/>
       <c r="K29" s="42"/>
     </row>
-    <row r="30" spans="1:11" s="93" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="110">
-        <v>42736</v>
-      </c>
-      <c r="B30" s="92"/>
-      <c r="C30" s="123" t="s">
+    <row r="30" spans="1:11" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B30" s="7"/>
+      <c r="C30" s="86" t="s">
         <v>285</v>
       </c>
-      <c r="D30" s="111" t="s">
-        <v>474</v>
-      </c>
-      <c r="E30" s="93" t="s">
+      <c r="D30" s="173" t="s">
+        <v>548</v>
+      </c>
+      <c r="E30" t="s">
         <v>271</v>
       </c>
-      <c r="F30" s="111" t="s">
+      <c r="F30" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="G30" s="92"/>
-      <c r="H30" s="92"/>
-      <c r="I30" s="92"/>
-      <c r="J30" s="92"/>
-      <c r="K30" s="92"/>
-    </row>
-    <row r="31" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B31" s="7"/>
+      <c r="G30" s="42"/>
+      <c r="H30" s="42"/>
+      <c r="I30" s="42"/>
+      <c r="J30" s="42"/>
+      <c r="K30" s="42"/>
+    </row>
+    <row r="31" spans="1:11" s="93" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="110">
+        <v>42736</v>
+      </c>
+      <c r="B31" s="92"/>
       <c r="C31" s="123" t="s">
         <v>285</v>
       </c>
-      <c r="D31" s="59" t="s">
-        <v>489</v>
-      </c>
-      <c r="E31" t="s">
+      <c r="D31" s="111" t="s">
+        <v>474</v>
+      </c>
+      <c r="E31" s="93" t="s">
         <v>271</v>
       </c>
-      <c r="F31" s="8" t="s">
+      <c r="F31" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7"/>
+      <c r="G31" s="92"/>
+      <c r="H31" s="92"/>
+      <c r="I31" s="92"/>
+      <c r="J31" s="92"/>
+      <c r="K31" s="92"/>
     </row>
     <row r="32" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="10">
@@ -13577,8 +13578,8 @@
       <c r="C32" s="123" t="s">
         <v>285</v>
       </c>
-      <c r="D32" s="57" t="s">
-        <v>478</v>
+      <c r="D32" s="59" t="s">
+        <v>489</v>
       </c>
       <c r="E32" t="s">
         <v>271</v>
@@ -13592,16 +13593,16 @@
       <c r="J32" s="7"/>
       <c r="K32" s="7"/>
     </row>
-    <row r="33" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="10">
         <v>42736</v>
       </c>
       <c r="B33" s="7"/>
-      <c r="C33" s="57" t="s">
-        <v>329</v>
+      <c r="C33" s="123" t="s">
+        <v>285</v>
       </c>
       <c r="D33" s="57" t="s">
-        <v>332</v>
+        <v>478</v>
       </c>
       <c r="E33" t="s">
         <v>271</v>
@@ -13609,7 +13610,7 @@
       <c r="F33" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="G33" s="8"/>
+      <c r="G33" s="7"/>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
       <c r="J33" s="7"/>
@@ -13619,12 +13620,12 @@
       <c r="A34" s="10">
         <v>42736</v>
       </c>
-      <c r="B34" s="10"/>
+      <c r="B34" s="7"/>
       <c r="C34" s="57" t="s">
         <v>329</v>
       </c>
       <c r="D34" s="57" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E34" t="s">
         <v>271</v>
@@ -13647,7 +13648,7 @@
         <v>329</v>
       </c>
       <c r="D35" s="57" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="E35" t="s">
         <v>271</v>
@@ -13670,7 +13671,7 @@
         <v>329</v>
       </c>
       <c r="D36" s="57" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="E36" t="s">
         <v>271</v>
@@ -13693,7 +13694,7 @@
         <v>329</v>
       </c>
       <c r="D37" s="57" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E37" t="s">
         <v>271</v>
@@ -13716,7 +13717,7 @@
         <v>329</v>
       </c>
       <c r="D38" s="57" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E38" t="s">
         <v>271</v>
@@ -13739,7 +13740,7 @@
         <v>329</v>
       </c>
       <c r="D39" s="57" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E39" t="s">
         <v>271</v>
@@ -13762,7 +13763,7 @@
         <v>329</v>
       </c>
       <c r="D40" s="57" t="s">
-        <v>364</v>
+        <v>338</v>
       </c>
       <c r="E40" t="s">
         <v>271</v>
@@ -13785,7 +13786,7 @@
         <v>329</v>
       </c>
       <c r="D41" s="57" t="s">
-        <v>348</v>
+        <v>364</v>
       </c>
       <c r="E41" t="s">
         <v>271</v>
@@ -13808,7 +13809,7 @@
         <v>329</v>
       </c>
       <c r="D42" s="57" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="E42" t="s">
         <v>271</v>
@@ -13822,51 +13823,51 @@
       <c r="J42" s="7"/>
       <c r="K42" s="7"/>
     </row>
-    <row r="43" spans="1:11" s="93" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="110">
-        <v>42736</v>
-      </c>
-      <c r="B43" s="110"/>
-      <c r="C43" s="112" t="s">
+    <row r="43" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B43" s="10"/>
+      <c r="C43" s="57" t="s">
         <v>329</v>
       </c>
-      <c r="D43" s="111" t="s">
+      <c r="D43" s="57" t="s">
+        <v>354</v>
+      </c>
+      <c r="E43" t="s">
+        <v>271</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="G43" s="8"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="7"/>
+      <c r="J43" s="7"/>
+      <c r="K43" s="7"/>
+    </row>
+    <row r="44" spans="1:11" s="93" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="110">
+        <v>42736</v>
+      </c>
+      <c r="B44" s="110"/>
+      <c r="C44" s="112" t="s">
+        <v>329</v>
+      </c>
+      <c r="D44" s="111" t="s">
         <v>474</v>
       </c>
-      <c r="E43" s="93" t="s">
+      <c r="E44" s="93" t="s">
         <v>271</v>
       </c>
-      <c r="F43" s="111" t="s">
+      <c r="F44" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="G43" s="111"/>
-      <c r="H43" s="115"/>
-      <c r="I43" s="115"/>
-      <c r="J43" s="115"/>
-      <c r="K43" s="115"/>
-    </row>
-    <row r="44" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B44" s="10"/>
-      <c r="C44" s="57" t="s">
-        <v>373</v>
-      </c>
-      <c r="D44" s="57" t="s">
-        <v>332</v>
-      </c>
-      <c r="E44" t="s">
-        <v>271</v>
-      </c>
-      <c r="F44" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="G44" s="8"/>
-      <c r="H44" s="7"/>
-      <c r="I44" s="7"/>
-      <c r="J44" s="7"/>
-      <c r="K44" s="7"/>
+      <c r="G44" s="111"/>
+      <c r="H44" s="115"/>
+      <c r="I44" s="115"/>
+      <c r="J44" s="115"/>
+      <c r="K44" s="115"/>
     </row>
     <row r="45" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="10">
@@ -13877,7 +13878,7 @@
         <v>373</v>
       </c>
       <c r="D45" s="57" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E45" t="s">
         <v>271</v>
@@ -13900,7 +13901,7 @@
         <v>373</v>
       </c>
       <c r="D46" s="57" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="E46" t="s">
         <v>271</v>
@@ -13923,7 +13924,7 @@
         <v>373</v>
       </c>
       <c r="D47" s="57" t="s">
-        <v>387</v>
+        <v>336</v>
       </c>
       <c r="E47" t="s">
         <v>271</v>
@@ -13937,97 +13938,97 @@
       <c r="J47" s="7"/>
       <c r="K47" s="7"/>
     </row>
-    <row r="48" spans="1:11" s="93" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="110">
-        <v>42736</v>
-      </c>
-      <c r="B48" s="110"/>
-      <c r="C48" s="112" t="s">
+    <row r="48" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A48" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B48" s="10"/>
+      <c r="C48" s="57" t="s">
         <v>373</v>
       </c>
-      <c r="D48" s="111" t="s">
+      <c r="D48" s="57" t="s">
+        <v>387</v>
+      </c>
+      <c r="E48" t="s">
+        <v>271</v>
+      </c>
+      <c r="F48" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="G48" s="8"/>
+      <c r="H48" s="7"/>
+      <c r="I48" s="7"/>
+      <c r="J48" s="7"/>
+      <c r="K48" s="7"/>
+    </row>
+    <row r="49" spans="1:11" s="93" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A49" s="110">
+        <v>42736</v>
+      </c>
+      <c r="B49" s="110"/>
+      <c r="C49" s="112" t="s">
+        <v>373</v>
+      </c>
+      <c r="D49" s="111" t="s">
         <v>474</v>
       </c>
-      <c r="E48" s="93" t="s">
+      <c r="E49" s="93" t="s">
         <v>271</v>
       </c>
-      <c r="F48" s="111" t="s">
+      <c r="F49" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="G48" s="111"/>
-      <c r="H48" s="115"/>
-      <c r="I48" s="115"/>
-      <c r="J48" s="115"/>
-      <c r="K48" s="115"/>
-    </row>
-    <row r="49" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B49" s="10"/>
-      <c r="C49" s="8" t="s">
+      <c r="G49" s="111"/>
+      <c r="H49" s="115"/>
+      <c r="I49" s="115"/>
+      <c r="J49" s="115"/>
+      <c r="K49" s="115"/>
+    </row>
+    <row r="50" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A50" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B50" s="10"/>
+      <c r="C50" s="8" t="s">
         <v>392</v>
       </c>
-      <c r="D49" s="8" t="s">
+      <c r="D50" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E50" t="s">
         <v>271</v>
       </c>
-      <c r="F49" s="8" t="s">
+      <c r="F50" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="G49" s="8"/>
-      <c r="H49" s="7"/>
-      <c r="I49" s="7"/>
-      <c r="J49" s="7"/>
-      <c r="K49" s="7"/>
-    </row>
-    <row r="50" spans="1:11" s="93" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="110">
-        <v>42736</v>
-      </c>
-      <c r="B50" s="110"/>
-      <c r="C50" s="111" t="s">
+      <c r="G50" s="8"/>
+      <c r="H50" s="7"/>
+      <c r="I50" s="7"/>
+      <c r="J50" s="7"/>
+      <c r="K50" s="7"/>
+    </row>
+    <row r="51" spans="1:11" s="93" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A51" s="110">
+        <v>42736</v>
+      </c>
+      <c r="B51" s="110"/>
+      <c r="C51" s="111" t="s">
         <v>392</v>
       </c>
-      <c r="D50" s="111" t="s">
+      <c r="D51" s="111" t="s">
         <v>474</v>
       </c>
-      <c r="E50" s="93" t="s">
+      <c r="E51" s="93" t="s">
         <v>271</v>
       </c>
-      <c r="F50" s="111" t="s">
+      <c r="F51" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="G50" s="111"/>
-      <c r="H50" s="115"/>
-      <c r="I50" s="115"/>
-      <c r="J50" s="115"/>
-      <c r="K50" s="115"/>
-    </row>
-    <row r="51" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B51" s="10"/>
-      <c r="C51" s="8" t="s">
-        <v>397</v>
-      </c>
-      <c r="D51" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="E51" t="s">
-        <v>271</v>
-      </c>
-      <c r="F51" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="G51" s="8"/>
-      <c r="H51" s="7"/>
-      <c r="I51" s="7"/>
-      <c r="J51" s="7"/>
-      <c r="K51" s="7"/>
+      <c r="G51" s="111"/>
+      <c r="H51" s="115"/>
+      <c r="I51" s="115"/>
+      <c r="J51" s="115"/>
+      <c r="K51" s="115"/>
     </row>
     <row r="52" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="10">
@@ -14037,8 +14038,8 @@
       <c r="C52" s="8" t="s">
         <v>397</v>
       </c>
-      <c r="D52" s="225" t="s">
-        <v>603</v>
+      <c r="D52" s="8" t="s">
+        <v>66</v>
       </c>
       <c r="E52" t="s">
         <v>271</v>
@@ -14060,8 +14061,8 @@
       <c r="C53" s="8" t="s">
         <v>397</v>
       </c>
-      <c r="D53" s="242" t="s">
-        <v>333</v>
+      <c r="D53" s="225" t="s">
+        <v>603</v>
       </c>
       <c r="E53" t="s">
         <v>271</v>
@@ -14084,7 +14085,7 @@
         <v>397</v>
       </c>
       <c r="D54" s="242" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="E54" t="s">
         <v>271</v>
@@ -14098,30 +14099,30 @@
       <c r="J54" s="7"/>
       <c r="K54" s="7"/>
     </row>
-    <row r="55" spans="1:11" s="146" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A55" s="197">
-        <v>42736</v>
-      </c>
-      <c r="B55" s="197"/>
-      <c r="C55" s="198" t="s">
+    <row r="55" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A55" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B55" s="10"/>
+      <c r="C55" s="8" t="s">
         <v>397</v>
       </c>
-      <c r="D55" s="198" t="s">
-        <v>580</v>
-      </c>
-      <c r="E55" s="199" t="s">
+      <c r="D55" s="242" t="s">
+        <v>336</v>
+      </c>
+      <c r="E55" t="s">
         <v>271</v>
       </c>
-      <c r="F55" s="198" t="s">
+      <c r="F55" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="G55" s="147"/>
-      <c r="H55" s="148"/>
-      <c r="I55" s="148"/>
-      <c r="J55" s="148"/>
-      <c r="K55" s="148"/>
-    </row>
-    <row r="56" spans="1:11" s="146" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G55" s="8"/>
+      <c r="H55" s="7"/>
+      <c r="I55" s="7"/>
+      <c r="J55" s="7"/>
+      <c r="K55" s="7"/>
+    </row>
+    <row r="56" spans="1:11" s="146" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="197">
         <v>42736</v>
       </c>
@@ -14130,7 +14131,7 @@
         <v>397</v>
       </c>
       <c r="D56" s="198" t="s">
-        <v>75</v>
+        <v>580</v>
       </c>
       <c r="E56" s="199" t="s">
         <v>271</v>
@@ -14138,6 +14139,11 @@
       <c r="F56" s="198" t="s">
         <v>244</v>
       </c>
+      <c r="G56" s="147"/>
+      <c r="H56" s="148"/>
+      <c r="I56" s="148"/>
+      <c r="J56" s="148"/>
+      <c r="K56" s="148"/>
     </row>
     <row r="57" spans="1:11" s="146" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="197">
@@ -14148,7 +14154,7 @@
         <v>397</v>
       </c>
       <c r="D57" s="198" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E57" s="199" t="s">
         <v>271</v>
@@ -14166,7 +14172,7 @@
         <v>397</v>
       </c>
       <c r="D58" s="198" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E58" s="199" t="s">
         <v>271</v>
@@ -14175,7 +14181,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="59" spans="1:11" s="167" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:11" s="146" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="197">
         <v>42736</v>
       </c>
@@ -14184,7 +14190,7 @@
         <v>397</v>
       </c>
       <c r="D59" s="198" t="s">
-        <v>270</v>
+        <v>83</v>
       </c>
       <c r="E59" s="199" t="s">
         <v>271</v>
@@ -14192,11 +14198,6 @@
       <c r="F59" s="198" t="s">
         <v>244</v>
       </c>
-      <c r="G59" s="169"/>
-      <c r="H59" s="170"/>
-      <c r="I59" s="170"/>
-      <c r="J59" s="170"/>
-      <c r="K59" s="170"/>
     </row>
     <row r="60" spans="1:11" s="167" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="197">
@@ -14207,7 +14208,7 @@
         <v>397</v>
       </c>
       <c r="D60" s="198" t="s">
-        <v>88</v>
+        <v>270</v>
       </c>
       <c r="E60" s="199" t="s">
         <v>271</v>
@@ -14221,39 +14222,44 @@
       <c r="J60" s="170"/>
       <c r="K60" s="170"/>
     </row>
-    <row r="61" spans="1:11" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A61" s="200">
-        <v>42736</v>
-      </c>
-      <c r="B61" s="200"/>
-      <c r="C61" s="201" t="s">
+    <row r="61" spans="1:11" s="167" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A61" s="197">
+        <v>42736</v>
+      </c>
+      <c r="B61" s="197"/>
+      <c r="C61" s="198" t="s">
         <v>397</v>
       </c>
-      <c r="D61" s="201" t="s">
+      <c r="D61" s="198" t="s">
+        <v>88</v>
+      </c>
+      <c r="E61" s="199" t="s">
+        <v>271</v>
+      </c>
+      <c r="F61" s="198" t="s">
+        <v>244</v>
+      </c>
+      <c r="G61" s="169"/>
+      <c r="H61" s="170"/>
+      <c r="I61" s="170"/>
+      <c r="J61" s="170"/>
+      <c r="K61" s="170"/>
+    </row>
+    <row r="62" spans="1:11" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A62" s="200">
+        <v>42736</v>
+      </c>
+      <c r="B62" s="200"/>
+      <c r="C62" s="201" t="s">
+        <v>397</v>
+      </c>
+      <c r="D62" s="201" t="s">
         <v>474</v>
       </c>
-      <c r="E61" s="202" t="s">
+      <c r="E62" s="202" t="s">
         <v>271</v>
       </c>
-      <c r="F61" s="201" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A62" s="197">
-        <v>42736</v>
-      </c>
-      <c r="B62" s="197"/>
-      <c r="C62" s="198" t="s">
-        <v>397</v>
-      </c>
-      <c r="D62" s="203" t="s">
-        <v>494</v>
-      </c>
-      <c r="E62" s="199" t="s">
-        <v>271</v>
-      </c>
-      <c r="F62" s="198" t="s">
+      <c r="F62" s="201" t="s">
         <v>244</v>
       </c>
     </row>
@@ -14265,8 +14271,8 @@
       <c r="C63" s="198" t="s">
         <v>397</v>
       </c>
-      <c r="D63" s="204" t="s">
-        <v>79</v>
+      <c r="D63" s="203" t="s">
+        <v>494</v>
       </c>
       <c r="E63" s="199" t="s">
         <v>271</v>
@@ -14284,7 +14290,7 @@
         <v>397</v>
       </c>
       <c r="D64" s="204" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="E64" s="199" t="s">
         <v>271</v>
@@ -14302,7 +14308,7 @@
         <v>397</v>
       </c>
       <c r="D65" s="204" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E65" s="199" t="s">
         <v>271</v>
@@ -14319,8 +14325,8 @@
       <c r="C66" s="198" t="s">
         <v>397</v>
       </c>
-      <c r="D66" s="203" t="s">
-        <v>581</v>
+      <c r="D66" s="204" t="s">
+        <v>68</v>
       </c>
       <c r="E66" s="199" t="s">
         <v>271</v>
@@ -14338,7 +14344,7 @@
         <v>397</v>
       </c>
       <c r="D67" s="203" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="E67" s="199" t="s">
         <v>271</v>
@@ -14356,7 +14362,7 @@
         <v>397</v>
       </c>
       <c r="D68" s="203" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="E68" s="199" t="s">
         <v>271</v>
@@ -14374,7 +14380,7 @@
         <v>397</v>
       </c>
       <c r="D69" s="203" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="E69" s="199" t="s">
         <v>271</v>
@@ -14392,7 +14398,7 @@
         <v>397</v>
       </c>
       <c r="D70" s="203" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="E70" s="199" t="s">
         <v>271</v>
@@ -14410,7 +14416,7 @@
         <v>397</v>
       </c>
       <c r="D71" s="203" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="E71" s="199" t="s">
         <v>271</v>
@@ -14428,7 +14434,7 @@
         <v>397</v>
       </c>
       <c r="D72" s="203" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="E72" s="199" t="s">
         <v>271</v>
@@ -14446,7 +14452,7 @@
         <v>397</v>
       </c>
       <c r="D73" s="203" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="E73" s="199" t="s">
         <v>271</v>
@@ -14464,7 +14470,7 @@
         <v>397</v>
       </c>
       <c r="D74" s="203" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="E74" s="199" t="s">
         <v>271</v>
@@ -14482,7 +14488,7 @@
         <v>397</v>
       </c>
       <c r="D75" s="203" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="E75" s="199" t="s">
         <v>271</v>
@@ -14492,20 +14498,20 @@
       </c>
     </row>
     <row r="76" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A76" s="205">
-        <v>42736</v>
-      </c>
-      <c r="B76" s="205"/>
-      <c r="C76" s="206" t="s">
+      <c r="A76" s="197">
+        <v>42736</v>
+      </c>
+      <c r="B76" s="197"/>
+      <c r="C76" s="198" t="s">
         <v>397</v>
       </c>
-      <c r="D76" s="207" t="s">
-        <v>591</v>
-      </c>
-      <c r="E76" s="208" t="s">
+      <c r="D76" s="203" t="s">
+        <v>590</v>
+      </c>
+      <c r="E76" s="199" t="s">
         <v>271</v>
       </c>
-      <c r="F76" s="206" t="s">
+      <c r="F76" s="198" t="s">
         <v>244</v>
       </c>
     </row>
@@ -14518,7 +14524,7 @@
         <v>397</v>
       </c>
       <c r="D77" s="207" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="E77" s="208" t="s">
         <v>271</v>
@@ -14528,20 +14534,20 @@
       </c>
     </row>
     <row r="78" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A78" s="197">
-        <v>42736</v>
-      </c>
-      <c r="B78" s="197"/>
-      <c r="C78" s="198" t="s">
+      <c r="A78" s="205">
+        <v>42736</v>
+      </c>
+      <c r="B78" s="205"/>
+      <c r="C78" s="206" t="s">
         <v>397</v>
       </c>
-      <c r="D78" s="203" t="s">
-        <v>520</v>
-      </c>
-      <c r="E78" s="199" t="s">
+      <c r="D78" s="207" t="s">
+        <v>592</v>
+      </c>
+      <c r="E78" s="208" t="s">
         <v>271</v>
       </c>
-      <c r="F78" s="198" t="s">
+      <c r="F78" s="206" t="s">
         <v>244</v>
       </c>
     </row>
@@ -14554,7 +14560,7 @@
         <v>397</v>
       </c>
       <c r="D79" s="203" t="s">
-        <v>478</v>
+        <v>520</v>
       </c>
       <c r="E79" s="199" t="s">
         <v>271</v>
@@ -14564,20 +14570,20 @@
       </c>
     </row>
     <row r="80" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A80" s="209">
-        <v>42736</v>
-      </c>
-      <c r="B80" s="209"/>
-      <c r="C80" s="210" t="s">
+      <c r="A80" s="197">
+        <v>42736</v>
+      </c>
+      <c r="B80" s="197"/>
+      <c r="C80" s="198" t="s">
         <v>397</v>
       </c>
-      <c r="D80" s="210" t="s">
-        <v>334</v>
-      </c>
-      <c r="E80" s="211" t="s">
+      <c r="D80" s="203" t="s">
+        <v>478</v>
+      </c>
+      <c r="E80" s="199" t="s">
         <v>271</v>
       </c>
-      <c r="F80" s="210" t="s">
+      <c r="F80" s="198" t="s">
         <v>244</v>
       </c>
     </row>
@@ -14590,7 +14596,7 @@
         <v>397</v>
       </c>
       <c r="D81" s="210" t="s">
-        <v>593</v>
+        <v>334</v>
       </c>
       <c r="E81" s="211" t="s">
         <v>271</v>
@@ -14608,7 +14614,7 @@
         <v>397</v>
       </c>
       <c r="D82" s="210" t="s">
-        <v>337</v>
+        <v>593</v>
       </c>
       <c r="E82" s="211" t="s">
         <v>271</v>
@@ -14626,7 +14632,7 @@
         <v>397</v>
       </c>
       <c r="D83" s="210" t="s">
-        <v>594</v>
+        <v>337</v>
       </c>
       <c r="E83" s="211" t="s">
         <v>271</v>
@@ -14643,8 +14649,8 @@
       <c r="C84" s="210" t="s">
         <v>397</v>
       </c>
-      <c r="D84" s="212" t="s">
-        <v>338</v>
+      <c r="D84" s="210" t="s">
+        <v>594</v>
       </c>
       <c r="E84" s="211" t="s">
         <v>271</v>
@@ -14662,7 +14668,7 @@
         <v>397</v>
       </c>
       <c r="D85" s="212" t="s">
-        <v>595</v>
+        <v>338</v>
       </c>
       <c r="E85" s="211" t="s">
         <v>271</v>
@@ -14680,7 +14686,7 @@
         <v>397</v>
       </c>
       <c r="D86" s="212" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="E86" s="211" t="s">
         <v>271</v>
@@ -14698,7 +14704,7 @@
         <v>397</v>
       </c>
       <c r="D87" s="212" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="E87" s="211" t="s">
         <v>271</v>
@@ -14716,7 +14722,7 @@
         <v>397</v>
       </c>
       <c r="D88" s="212" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E88" s="211" t="s">
         <v>271</v>
@@ -14726,20 +14732,20 @@
       </c>
     </row>
     <row r="89" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A89" s="241">
-        <v>42736</v>
-      </c>
-      <c r="B89" s="241"/>
-      <c r="C89" s="258" t="s">
-        <v>602</v>
-      </c>
-      <c r="D89" s="242" t="s">
-        <v>296</v>
-      </c>
-      <c r="E89" s="245" t="s">
+      <c r="A89" s="209">
+        <v>42736</v>
+      </c>
+      <c r="B89" s="209"/>
+      <c r="C89" s="210" t="s">
+        <v>397</v>
+      </c>
+      <c r="D89" s="212" t="s">
+        <v>598</v>
+      </c>
+      <c r="E89" s="211" t="s">
         <v>271</v>
       </c>
-      <c r="F89" s="225" t="s">
+      <c r="F89" s="210" t="s">
         <v>244</v>
       </c>
     </row>
@@ -14752,7 +14758,7 @@
         <v>602</v>
       </c>
       <c r="D90" s="242" t="s">
-        <v>314</v>
+        <v>296</v>
       </c>
       <c r="E90" s="245" t="s">
         <v>271</v>
@@ -14770,7 +14776,7 @@
         <v>602</v>
       </c>
       <c r="D91" s="242" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E91" s="245" t="s">
         <v>271</v>
@@ -14783,12 +14789,12 @@
       <c r="A92" s="241">
         <v>42736</v>
       </c>
-      <c r="B92" s="245"/>
+      <c r="B92" s="241"/>
       <c r="C92" s="258" t="s">
         <v>602</v>
       </c>
       <c r="D92" s="242" t="s">
-        <v>454</v>
+        <v>311</v>
       </c>
       <c r="E92" s="245" t="s">
         <v>271</v>
@@ -14801,12 +14807,12 @@
       <c r="A93" s="241">
         <v>42736</v>
       </c>
-      <c r="B93" s="246"/>
+      <c r="B93" s="245"/>
       <c r="C93" s="258" t="s">
         <v>602</v>
       </c>
-      <c r="D93" s="258" t="s">
-        <v>474</v>
+      <c r="D93" s="242" t="s">
+        <v>454</v>
       </c>
       <c r="E93" s="245" t="s">
         <v>271</v>
@@ -14819,12 +14825,12 @@
       <c r="A94" s="241">
         <v>42736</v>
       </c>
-      <c r="B94" s="245"/>
+      <c r="B94" s="246"/>
       <c r="C94" s="258" t="s">
         <v>602</v>
       </c>
       <c r="D94" s="258" t="s">
-        <v>489</v>
+        <v>474</v>
       </c>
       <c r="E94" s="245" t="s">
         <v>271</v>
@@ -14842,12 +14848,30 @@
         <v>602</v>
       </c>
       <c r="D95" s="258" t="s">
-        <v>478</v>
+        <v>489</v>
       </c>
       <c r="E95" s="245" t="s">
         <v>271</v>
       </c>
       <c r="F95" s="225" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A96" s="241">
+        <v>42736</v>
+      </c>
+      <c r="B96" s="245"/>
+      <c r="C96" s="258" t="s">
+        <v>602</v>
+      </c>
+      <c r="D96" s="258" t="s">
+        <v>478</v>
+      </c>
+      <c r="E96" s="245" t="s">
+        <v>271</v>
+      </c>
+      <c r="F96" s="225" t="s">
         <v>244</v>
       </c>
     </row>

</xml_diff>